<commit_message>
CM17: Changes done in log4j and bugfixes..
</commit_message>
<xml_diff>
--- a/files/UserData.xlsx
+++ b/files/UserData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shubhangi_bhalerao\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace-MyBank\mybankTesting\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85C641E-A30E-4358-B75C-FD2B2D15C46C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC30200-2E85-4A09-B47F-579FE8732206}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9C2F40CB-1BF3-46C5-B44A-554F45661B4D}"/>
+    <workbookView xWindow="10930" yWindow="-1720" windowWidth="15600" windowHeight="10200" xr2:uid="{9C2F40CB-1BF3-46C5-B44A-554F45661B4D}"/>
   </bookViews>
   <sheets>
     <sheet name="correctdata" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t>Email Id</t>
   </si>
@@ -82,16 +82,109 @@
     <t>sachin@mail.com</t>
   </si>
   <si>
-    <t>c1shayan@gmail.com</t>
-  </si>
-  <si>
-    <t>g1aa@gmail.com</t>
-  </si>
-  <si>
-    <t>Cshayan@gmail.com</t>
-  </si>
-  <si>
-    <t>Caa@gmail.com</t>
+    <t>sakshi@reddif.com</t>
+  </si>
+  <si>
+    <t>Amit@gmail.com</t>
+  </si>
+  <si>
+    <t>kunal@gmail.com</t>
+  </si>
+  <si>
+    <t>pas123</t>
+  </si>
+  <si>
+    <t>yash3344@gmail.com</t>
+  </si>
+  <si>
+    <t>pass334</t>
+  </si>
+  <si>
+    <t>ankit@33.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>yash123</t>
+  </si>
+  <si>
+    <t>bbbb</t>
+  </si>
+  <si>
+    <t>none12</t>
+  </si>
+  <si>
+    <t>sapp</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>p123s</t>
+  </si>
+  <si>
+    <t>p55word</t>
+  </si>
+  <si>
+    <t>cyan@gmail.com</t>
+  </si>
+  <si>
+    <t>gaaaaa@gmail.com</t>
+  </si>
+  <si>
+    <t>sayantaaan1999arka@gmail.com</t>
+  </si>
+  <si>
+    <t>shayandff90@gmail.com</t>
+  </si>
+  <si>
+    <t>abc@ghmmail.com</t>
+  </si>
+  <si>
+    <t>juli@haaa.com</t>
+  </si>
+  <si>
+    <t>Jhon@vmail.com</t>
+  </si>
+  <si>
+    <t>shubhanYasgi@gmail.com</t>
+  </si>
+  <si>
+    <t>Gaa@gmail.com</t>
+  </si>
+  <si>
+    <t>Sayantan1999arka@gmail.com</t>
+  </si>
+  <si>
+    <t>ABC@gmail.com</t>
+  </si>
+  <si>
+    <t>JUli@aa.com</t>
+  </si>
+  <si>
+    <t>JHon@gmail.com</t>
+  </si>
+  <si>
+    <t>SHubhangi@gmail.com</t>
+  </si>
+  <si>
+    <t>csGHayan@gmail.com</t>
+  </si>
+  <si>
+    <t>Ankita@gmail.com</t>
+  </si>
+  <si>
+    <t>ashish@gmail.com</t>
+  </si>
+  <si>
+    <t>mayur@gmail.com</t>
+  </si>
+  <si>
+    <t>apurba@gmail.com</t>
+  </si>
+  <si>
+    <t>bhai@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -166,7 +259,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -485,16 +578,16 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.90625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" style="4"/>
+    <col min="1" max="1" width="26.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -502,223 +595,267 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C8810C0-B019-4C6E-B1A3-AF70D40FCF6A}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>23123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>1234</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{69318688-C313-413E-AA0F-D8A627FBBD10}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{AC824CAA-F306-41F8-AF57-3F0A7A934D6C}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{54E0A64F-F96D-4814-85E1-B73722C54C80}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{98823038-20A0-4261-B35B-4DDBB1A40394}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{1B7B53AE-5E61-4638-998B-E8547049ECD9}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{F354EF65-09F3-4F54-A394-6D833BDF71FE}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{D4BCB109-168B-41F3-B766-8BF2C16266D7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1DC8265-4167-4E5D-8539-CB48B41BFC64}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B2" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B3" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B6" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B7" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="4">
-        <v>1234</v>
+      <c r="B9" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" xr:uid="{E89F6353-DBD0-4DE5-9744-2BC7AA572300}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C8810C0-B019-4C6E-B1A3-AF70D40FCF6A}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="18.7265625" style="6" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2">
-        <v>1234</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{69318688-C313-413E-AA0F-D8A627FBBD10}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{AC824CAA-F306-41F8-AF57-3F0A7A934D6C}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1DC8265-4167-4E5D-8539-CB48B41BFC64}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="20.26953125" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="4">
-        <v>12343</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4">
-        <v>12343</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F144FB3-0898-4B8E-A22D-95D38D45702B}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="22.90625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1234</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{54284A17-57F6-4A48-957B-38F458138100}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{61874752-58C3-4029-B936-87FAD4C1060C}"/>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{054200B5-C423-4128-9961-1EC6D7D5DA76}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C1F2AFE-6BAE-406D-9C7B-020CAE5A748D}">
-  <dimension ref="A1:B3"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F144FB3-0898-4B8E-A22D-95D38D45702B}">
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7265625" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -726,32 +863,192 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B2" s="4">
         <v>1234</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B3" s="4">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="4">
         <v>1234</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{8275AAEB-04BF-4EAD-9FFD-AF0DD71A4D6C}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{A8E14072-09B8-44B0-B674-20043C15152A}"/>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{F93E84FD-2C5C-49C0-B966-FD2C66E90B7B}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{DB8EC80A-58FF-41D3-9C4F-07D16F952CFE}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{14D7D6FB-08F2-4FA9-A7C6-E3184730D73F}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{22C559AD-822B-4906-9AC9-A2A0F34A8780}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{E5352B8A-3275-48A0-A105-DEF28435D7EC}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{17BD610A-4576-4F6D-B412-8869964A68E3}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{1EB25914-B837-42A3-9C9D-4EE42DFE06DA}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{26335688-31F9-4955-8007-4C16A67E4D80}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C1F2AFE-6BAE-406D-9C7B-020CAE5A748D}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1234</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{420612BD-FF2D-414B-A709-FF72133C347A}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{A4005923-4AD8-4963-92B0-52F9C015F532}"/>
+    <hyperlink ref="A6" r:id="rId3" xr:uid="{D0483E3F-8852-436C-9FFF-466F7945BE99}"/>
+    <hyperlink ref="A7" r:id="rId4" xr:uid="{B657D35E-98CC-4077-83A7-2A07DD341E8D}"/>
+    <hyperlink ref="A8" r:id="rId5" xr:uid="{3FA86091-6A39-4AD8-9898-DAA2CDDEB0AD}"/>
+    <hyperlink ref="A9" r:id="rId6" xr:uid="{847365B9-9CB4-4E11-9431-743140537580}"/>
+    <hyperlink ref="A2" r:id="rId7" xr:uid="{1270E8FC-58B6-4589-9B21-F72872239FD9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -760,7 +1057,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002FC2FF12A2FF034D89A9B935048849AA" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dc89c257c8340e600a0bbd99ef76a478">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e7dcaecb-bb17-4f82-8dbb-4f6695320fa2" xmlns:ns4="4b6642a2-7e49-486b-9495-1b046d398585" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="93dc676102cdf92e5220f18f73fe0c3c" ns3:_="" ns4:_="">
     <xsd:import namespace="e7dcaecb-bb17-4f82-8dbb-4f6695320fa2"/>
@@ -957,13 +1254,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D5F5FD3-717B-49C5-A66B-70DD1A9E76FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="4b6642a2-7e49-486b-9495-1b046d398585"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="e7dcaecb-bb17-4f82-8dbb-4f6695320fa2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95695381-CD47-43BF-8291-336FF895D3C7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -971,7 +1279,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB7DF897-5805-4F0C-9410-D34BBE309361}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -988,21 +1296,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D5F5FD3-717B-49C5-A66B-70DD1A9E76FB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="4b6642a2-7e49-486b-9495-1b046d398585"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="e7dcaecb-bb17-4f82-8dbb-4f6695320fa2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>